<commit_message>
datasets britains species and golden gate added
</commit_message>
<xml_diff>
--- a/external_data/snakes.xlsx
+++ b/external_data/snakes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michiel/Rprojects/bintestr/external_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michiel/Rprojects/bindata/external_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F030AE-A212-184E-833A-A16B401104CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7440CC29-A848-484E-87CA-DE64CEB0A060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{CF4D9D45-C97B-6D41-96AC-CA38102FAC0C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{0CF10CCF-57DD-E34B-A016-4147E18B5C94}" name="bij2001-sup-0001-si" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/michiel/Rprojects/bintestr/external_data/bij2001-sup-0001-si.txt" decimal="," thousands="." tab="0" space="1" consecutive="1">
+    <textPr sourceFile="/Users/michiel/Rprojects/bintestr/external_data/bij2001-sup-0001-si.txt" decimal="," thousands="." tab="0" space="1" consecutive="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -3720,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7454236-76E2-7642-904D-8965D9419123}">
   <dimension ref="A2:E1478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="A678" sqref="A678"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>